<commit_message>
Run for California dataset
</commit_message>
<xml_diff>
--- a/results/CA/embedding_size_results.xlsx
+++ b/results/CA/embedding_size_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8240446693900854</v>
+        <v>0.8279476871118658</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8270578812257356</v>
+        <v>0.8281712605073157</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8238575883803874</v>
+        <v>0.8278746192363403</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8301967485070183</v>
+        <v>0.8282773431781433</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8317189564959502</v>
+        <v>0.8300777276889197</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8309369615063318</v>
+        <v>0.8332427783193037</v>
       </c>
     </row>
     <row r="8">
@@ -498,15 +498,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8298387116706346</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>30</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.8289910097286896</v>
+        <v>0.8306366459920242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>